<commit_message>
added result of spinReels to game
</commit_message>
<xml_diff>
--- a/Assets/images/ImageMap.xlsx
+++ b/Assets/images/ImageMap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -53,13 +53,13 @@
     <t>SpinButton</t>
   </si>
   <si>
-    <t>Reel 1</t>
-  </si>
-  <si>
-    <t>Reel 2</t>
-  </si>
-  <si>
-    <t>Reel 3</t>
+    <t>Image 1</t>
+  </si>
+  <si>
+    <t>Image 2</t>
+  </si>
+  <si>
+    <t>Image 3</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E8" s="2">
         <v>220</v>

</xml_diff>